<commit_message>
Arregla modelos, otros arreglos
</commit_message>
<xml_diff>
--- a/project/static/import/templates/DatoObjetivo.xlsx
+++ b/project/static/import/templates/DatoObjetivo.xlsx
@@ -22,6 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
+    <t xml:space="preserve">deportista</t>
+  </si>
+  <si>
     <t xml:space="preserve">evento</t>
   </si>
   <si>
@@ -65,9 +68,6 @@
   </si>
   <si>
     <t xml:space="preserve">eee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deportista</t>
   </si>
 </sst>
 </file>
@@ -189,13 +189,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -246,11 +246,11 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -263,11 +263,11 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -280,6 +280,7 @@
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Actualiza templates, agrega carga múltiple de deportistas (no funciona)
</commit_message>
<xml_diff>
--- a/project/static/import/templates/DatoObjetivo.xlsx
+++ b/project/static/import/templates/DatoObjetivo.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Datos Objetivos" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -192,10 +192,10 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Arregla importación de datos objetivos, otros fixs
</commit_message>
<xml_diff>
--- a/project/static/import/templates/DatoObjetivo.xlsx
+++ b/project/static/import/templates/DatoObjetivo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">deportista</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">velEntre20y25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">velMayor25</t>
   </si>
   <si>
     <t xml:space="preserve">acceleration</t>
@@ -192,10 +195,10 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -246,7 +249,9 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0"/>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2"/>

</xml_diff>